<commit_message>
Adds some climate data.
</commit_message>
<xml_diff>
--- a/contaminantsSortable.xlsx
+++ b/contaminantsSortable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfulmer\repos\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DD4449-D575-4891-8EF2-DF11E6151758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA6E10B-DABA-4676-82CF-DC54BC588295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{12F4FB9E-74FF-4D65-85C2-6F3C82155948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12F4FB9E-74FF-4D65-85C2-6F3C82155948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Benton</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Bentonville</t>
   </si>
   <si>
-    <t>&lt; 2,000</t>
-  </si>
-  <si>
-    <t>&lt; 4,000</t>
-  </si>
-  <si>
     <t>Crawford</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>Total Contaminants</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Sheridan</t>
   </si>
 </sst>
 </file>
@@ -589,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFA1530-CD47-4561-84F5-DFCBA0F6C8A4}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,81 +608,81 @@
   <sheetData>
     <row r="1" spans="1:7" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2000</v>
       </c>
       <c r="E2" s="1">
         <v>123</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="4">
         <f>SUM(C2,D2,E2)</f>
-        <v>123</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4">
-        <v>5309</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1">
+        <v>871</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>38</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G3" s="4">
         <f>SUM(C3,D3,E3)</f>
-        <v>5309</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>7377</v>
@@ -691,7 +691,7 @@
         <v>166</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2">
         <v>1334</v>
@@ -703,271 +703,295 @@
     </row>
     <row r="5" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4">
-        <v>13000</v>
+        <v>4000</v>
       </c>
       <c r="D5" s="4">
-        <v>7463</v>
-      </c>
-      <c r="E5" s="3">
-        <v>198</v>
+        <v>5309</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G5" s="4">
         <f>SUM(C5,D5,E5)</f>
-        <v>20661</v>
+        <v>9309</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4">
-        <v>5611</v>
+        <v>13000</v>
       </c>
       <c r="D6" s="4">
-        <v>35524</v>
+        <v>7463</v>
       </c>
       <c r="E6" s="3">
-        <v>20</v>
+        <v>198</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4">
         <f>SUM(C6,D6,E6)</f>
-        <v>41155</v>
+        <v>20661</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4">
-        <v>6400</v>
+        <v>5611</v>
       </c>
       <c r="D7" s="4">
-        <v>40850</v>
+        <v>35524</v>
       </c>
       <c r="E7" s="3">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G7" s="4">
         <f>SUM(C7,D7,E7)</f>
-        <v>47416</v>
+        <v>41155</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="2">
-        <v>114295</v>
-      </c>
-      <c r="E8" s="1">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6400</v>
+      </c>
+      <c r="D8" s="4">
+        <v>40850</v>
+      </c>
+      <c r="E8" s="3">
+        <v>166</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="G8" s="4">
         <f>SUM(C8,D8,E8)</f>
-        <v>119307</v>
+        <v>47416</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2">
-        <v>14400</v>
+        <v>5000</v>
       </c>
       <c r="D9" s="2">
-        <v>185682</v>
-      </c>
-      <c r="E9" s="2">
-        <v>4041</v>
+        <v>114295</v>
+      </c>
+      <c r="E9" s="1">
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G9" s="4">
         <f>SUM(C9,D9,E9)</f>
-        <v>204123</v>
+        <v>119307</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4">
-        <v>227708</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>15</v>
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2">
+        <v>14400</v>
+      </c>
+      <c r="D10" s="2">
+        <v>185682</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4041</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G10" s="4">
         <f>SUM(C10,D10,E10)</f>
-        <v>227708</v>
+        <v>204123</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>227708</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="4">
-        <v>263000</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G11" s="4">
         <f>SUM(C11,D11,E11)</f>
+        <v>227708</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4">
         <v>263000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8607</v>
-      </c>
-      <c r="D12" s="2">
-        <v>267602</v>
-      </c>
-      <c r="E12" s="1">
-        <v>126</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>6</v>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="G12" s="4">
         <f>SUM(C12,D12,E12)</f>
-        <v>276335</v>
+        <v>263000</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8607</v>
       </c>
       <c r="D13" s="2">
-        <v>344816</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2074</v>
+        <v>267602</v>
+      </c>
+      <c r="E13" s="1">
+        <v>126</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G13" s="4">
         <f>SUM(C13,D13,E13)</f>
+        <v>276335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2">
         <v>344816</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D14" s="4">
-        <v>643510</v>
-      </c>
-      <c r="E14" s="4">
-        <v>5719</v>
-      </c>
-      <c r="F14" s="3">
-        <v>886</v>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2074</v>
       </c>
       <c r="G14" s="4">
         <f>SUM(C14,D14,E14)</f>
-        <v>651229</v>
+        <v>344816</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>818311</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="2">
-        <v>2793</v>
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2000</v>
+      </c>
+      <c r="D15" s="4">
+        <v>643510</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5719</v>
+      </c>
+      <c r="F15" s="3">
+        <v>886</v>
       </c>
       <c r="G15" s="4">
         <f>SUM(C15,D15,E15)</f>
+        <v>651229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D16" s="2">
         <v>818311</v>
       </c>
+      <c r="E16" s="2">
+        <v>4000</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2793</v>
+      </c>
+      <c r="G16" s="4">
+        <f>SUM(C16,D16,E16)</f>
+        <v>824311</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G18">
-    <sortCondition ref="G1:G18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
+    <sortCondition ref="G1:G16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>